<commit_message>
Edited pitch config input.
</commit_message>
<xml_diff>
--- a/OpenVEHICLE_sheet_OJ.xlsx
+++ b/OpenVEHICLE_sheet_OJ.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ojeif\OneDrive\Documents\MATLAB\OpenLAP-Lap-Time-Simulator\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ojeif\OneDrive\Documents\Formula\VD-FOMRULA-ELECTRIC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{396AC558-488D-47B6-ACE3-0F9AA83036E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAC3DE2C-EE93-4C16-A485-D658408862A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3450" yWindow="4245" windowWidth="21600" windowHeight="11235" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" r:id="rId1"/>
@@ -100,262 +100,262 @@
     <t>Brakes</t>
   </si>
   <si>
+    <t>Air Density</t>
+  </si>
+  <si>
+    <t>Disc Outer Diameter</t>
+  </si>
+  <si>
+    <t>Pad Height</t>
+  </si>
+  <si>
+    <t>Caliper Number of Pistons</t>
+  </si>
+  <si>
+    <t>Caliper Piston Diameter</t>
+  </si>
+  <si>
+    <t>Master Cylinder Piston Diameter</t>
+  </si>
+  <si>
+    <t>Pedal Ratio</t>
+  </si>
+  <si>
+    <t>Tyres</t>
+  </si>
+  <si>
+    <t>Tyre Radius</t>
+  </si>
+  <si>
+    <t>Longitudinal Friction Coefficient</t>
+  </si>
+  <si>
+    <t>Longitudinal Friction Load Rating</t>
+  </si>
+  <si>
+    <t>Longitudinal Friction Sensitivity</t>
+  </si>
+  <si>
+    <t>1/N</t>
+  </si>
+  <si>
+    <t>Rolling Resistance</t>
+  </si>
+  <si>
+    <t>Grip Factor Multiplier</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Lateral Friction Coefficient</t>
+  </si>
+  <si>
+    <t>Lateral Friction Load Rating</t>
+  </si>
+  <si>
+    <t>Lateral Friction Sensitivity</t>
+  </si>
+  <si>
+    <t>Front Cornering Stiffness</t>
+  </si>
+  <si>
+    <t>Rear Cornering Stiffness</t>
+  </si>
+  <si>
+    <t>N/deg</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>Unit</t>
+  </si>
+  <si>
+    <t>Comment</t>
+  </si>
+  <si>
+    <t>Engine</t>
+  </si>
+  <si>
+    <t>Power Factor Multiplier</t>
+  </si>
+  <si>
+    <t>Thermal Efficiency</t>
+  </si>
+  <si>
+    <t>Fuel Lower Heating Value</t>
+  </si>
+  <si>
+    <t>J/kg</t>
+  </si>
+  <si>
+    <t>Transmission</t>
+  </si>
+  <si>
+    <t>Drive Type</t>
+  </si>
+  <si>
+    <t>[Steering Wheel Angle]/[Wheel Angle]</t>
+  </si>
+  <si>
+    <t>[Foot Force Application Point Lever Arm]/[Master Cylinder Lever Arm]</t>
+  </si>
+  <si>
+    <t>Primary Gear Reduction</t>
+  </si>
+  <si>
+    <t>Final Gear Reduction</t>
+  </si>
+  <si>
+    <t>1st Gear Ratio</t>
+  </si>
+  <si>
+    <t>2nd Gear Ratio</t>
+  </si>
+  <si>
+    <t>3rd Gear Ratio</t>
+  </si>
+  <si>
+    <t>4th Gear Ratio</t>
+  </si>
+  <si>
+    <t>5th Gear Ratio</t>
+  </si>
+  <si>
+    <t>6th Gear Ratio</t>
+  </si>
+  <si>
+    <t>7th Gear Ratio</t>
+  </si>
+  <si>
+    <t>8th Gear Ratio</t>
+  </si>
+  <si>
+    <t>9th Gear Ratio</t>
+  </si>
+  <si>
+    <t>10th Gear Ratio</t>
+  </si>
+  <si>
+    <t>Front Aero Distribution</t>
+  </si>
+  <si>
+    <t>Lift Coefficient CL</t>
+  </si>
+  <si>
+    <t>Drag Coefficient CD</t>
+  </si>
+  <si>
+    <t>Primary Gear Efficiency</t>
+  </si>
+  <si>
+    <t>Final Gear Efficiency</t>
+  </si>
+  <si>
+    <t>Gearbox Efficiency</t>
+  </si>
+  <si>
+    <t>Pad Friction Coefficient</t>
+  </si>
+  <si>
+    <t>Gear Shift Time</t>
+  </si>
+  <si>
+    <t>s</t>
+  </si>
+  <si>
+    <t>Only used in dragster mode</t>
+  </si>
+  <si>
+    <t>Assumed to be the same on all pads. Recommended value: 0.45</t>
+  </si>
+  <si>
+    <t>Recommended value:  800-1000</t>
+  </si>
+  <si>
+    <t>Assumed to be the same on all tyres. Should be positive. Recommended value:  0.0001</t>
+  </si>
+  <si>
+    <t>Recommended value:  1.225</t>
+  </si>
+  <si>
+    <t>Should be negative</t>
+  </si>
+  <si>
+    <t>Positive = Lift / Negative = Downforce</t>
+  </si>
+  <si>
+    <t>Recommended value:  0.90 for bevel gears</t>
+  </si>
+  <si>
+    <t>Recommended value:  0.98 for spur/helical gears</t>
+  </si>
+  <si>
+    <t>Assumed to be the same on all tyres. Recommended value: M/4</t>
+  </si>
+  <si>
+    <t>Assumed to be the same on all tyres. Slick tyres: 1.8, Street tyres: 0.9-1.2</t>
+  </si>
+  <si>
+    <t>Assumed to be the same on all tyres. Needs to be negative. Recommended value: -0.001</t>
+  </si>
+  <si>
+    <t>Assumed to be the same on all tyres.</t>
+  </si>
+  <si>
+    <t>Assumed to be the same on all corners.</t>
+  </si>
+  <si>
+    <t>Assumed to be the same both front and rear.</t>
+  </si>
+  <si>
+    <t>Recommended value: 0.3 for ICE</t>
+  </si>
+  <si>
+    <t>Recommended value:  4.72E+07 for petrol</t>
+  </si>
+  <si>
+    <t>From crancskaft to Input shaft.</t>
+  </si>
+  <si>
+    <t>EV7</t>
+  </si>
+  <si>
+    <t>Open Wheel</t>
+  </si>
+  <si>
+    <t>Weight Distr W 68kg Driver Front</t>
+  </si>
+  <si>
+    <t>RWD</t>
+  </si>
+  <si>
+    <t>Configuration</t>
+  </si>
+  <si>
+    <t>CL</t>
+  </si>
+  <si>
+    <t>CD</t>
+  </si>
+  <si>
+    <t>Pitch Front</t>
+  </si>
+  <si>
+    <t>Pitch Rear</t>
+  </si>
+  <si>
     <t>CL Scale Multiplier</t>
   </si>
   <si>
     <t>CD Scale Multiplier</t>
-  </si>
-  <si>
-    <t>Air Density</t>
-  </si>
-  <si>
-    <t>Disc Outer Diameter</t>
-  </si>
-  <si>
-    <t>Pad Height</t>
-  </si>
-  <si>
-    <t>Caliper Number of Pistons</t>
-  </si>
-  <si>
-    <t>Caliper Piston Diameter</t>
-  </si>
-  <si>
-    <t>Master Cylinder Piston Diameter</t>
-  </si>
-  <si>
-    <t>Pedal Ratio</t>
-  </si>
-  <si>
-    <t>Tyres</t>
-  </si>
-  <si>
-    <t>Tyre Radius</t>
-  </si>
-  <si>
-    <t>Longitudinal Friction Coefficient</t>
-  </si>
-  <si>
-    <t>Longitudinal Friction Load Rating</t>
-  </si>
-  <si>
-    <t>Longitudinal Friction Sensitivity</t>
-  </si>
-  <si>
-    <t>1/N</t>
-  </si>
-  <si>
-    <t>Rolling Resistance</t>
-  </si>
-  <si>
-    <t>Grip Factor Multiplier</t>
-  </si>
-  <si>
-    <t>-</t>
-  </si>
-  <si>
-    <t>Lateral Friction Coefficient</t>
-  </si>
-  <si>
-    <t>Lateral Friction Load Rating</t>
-  </si>
-  <si>
-    <t>Lateral Friction Sensitivity</t>
-  </si>
-  <si>
-    <t>Front Cornering Stiffness</t>
-  </si>
-  <si>
-    <t>Rear Cornering Stiffness</t>
-  </si>
-  <si>
-    <t>N/deg</t>
-  </si>
-  <si>
-    <t>Category</t>
-  </si>
-  <si>
-    <t>Description</t>
-  </si>
-  <si>
-    <t>Value</t>
-  </si>
-  <si>
-    <t>Unit</t>
-  </si>
-  <si>
-    <t>Comment</t>
-  </si>
-  <si>
-    <t>Engine</t>
-  </si>
-  <si>
-    <t>Power Factor Multiplier</t>
-  </si>
-  <si>
-    <t>Thermal Efficiency</t>
-  </si>
-  <si>
-    <t>Fuel Lower Heating Value</t>
-  </si>
-  <si>
-    <t>J/kg</t>
-  </si>
-  <si>
-    <t>Transmission</t>
-  </si>
-  <si>
-    <t>Drive Type</t>
-  </si>
-  <si>
-    <t>[Steering Wheel Angle]/[Wheel Angle]</t>
-  </si>
-  <si>
-    <t>[Foot Force Application Point Lever Arm]/[Master Cylinder Lever Arm]</t>
-  </si>
-  <si>
-    <t>Primary Gear Reduction</t>
-  </si>
-  <si>
-    <t>Final Gear Reduction</t>
-  </si>
-  <si>
-    <t>1st Gear Ratio</t>
-  </si>
-  <si>
-    <t>2nd Gear Ratio</t>
-  </si>
-  <si>
-    <t>3rd Gear Ratio</t>
-  </si>
-  <si>
-    <t>4th Gear Ratio</t>
-  </si>
-  <si>
-    <t>5th Gear Ratio</t>
-  </si>
-  <si>
-    <t>6th Gear Ratio</t>
-  </si>
-  <si>
-    <t>7th Gear Ratio</t>
-  </si>
-  <si>
-    <t>8th Gear Ratio</t>
-  </si>
-  <si>
-    <t>9th Gear Ratio</t>
-  </si>
-  <si>
-    <t>10th Gear Ratio</t>
-  </si>
-  <si>
-    <t>Front Aero Distribution</t>
-  </si>
-  <si>
-    <t>Lift Coefficient CL</t>
-  </si>
-  <si>
-    <t>Drag Coefficient CD</t>
-  </si>
-  <si>
-    <t>Primary Gear Efficiency</t>
-  </si>
-  <si>
-    <t>Final Gear Efficiency</t>
-  </si>
-  <si>
-    <t>Gearbox Efficiency</t>
-  </si>
-  <si>
-    <t>Pad Friction Coefficient</t>
-  </si>
-  <si>
-    <t>Gear Shift Time</t>
-  </si>
-  <si>
-    <t>s</t>
-  </si>
-  <si>
-    <t>Only used in dragster mode</t>
-  </si>
-  <si>
-    <t>Assumed to be the same on all pads. Recommended value: 0.45</t>
-  </si>
-  <si>
-    <t>Recommended value:  800-1000</t>
-  </si>
-  <si>
-    <t>Assumed to be the same on all tyres. Should be positive. Recommended value:  0.0001</t>
-  </si>
-  <si>
-    <t>Recommended value:  1.225</t>
-  </si>
-  <si>
-    <t>Should be negative</t>
-  </si>
-  <si>
-    <t>Positive = Lift / Negative = Downforce</t>
-  </si>
-  <si>
-    <t>Recommended value:  0.90 for bevel gears</t>
-  </si>
-  <si>
-    <t>Recommended value:  0.98 for spur/helical gears</t>
-  </si>
-  <si>
-    <t>Assumed to be the same on all tyres. Recommended value: M/4</t>
-  </si>
-  <si>
-    <t>Assumed to be the same on all tyres. Slick tyres: 1.8, Street tyres: 0.9-1.2</t>
-  </si>
-  <si>
-    <t>Assumed to be the same on all tyres. Needs to be negative. Recommended value: -0.001</t>
-  </si>
-  <si>
-    <t>Assumed to be the same on all tyres.</t>
-  </si>
-  <si>
-    <t>Assumed to be the same on all corners.</t>
-  </si>
-  <si>
-    <t>Assumed to be the same both front and rear.</t>
-  </si>
-  <si>
-    <t>Recommended value: 0.3 for ICE</t>
-  </si>
-  <si>
-    <t>Recommended value:  4.72E+07 for petrol</t>
-  </si>
-  <si>
-    <t>From crancskaft to Input shaft.</t>
-  </si>
-  <si>
-    <t>EV7</t>
-  </si>
-  <si>
-    <t>Open Wheel</t>
-  </si>
-  <si>
-    <t>Weight Distr W 68kg Driver Front</t>
-  </si>
-  <si>
-    <t>RWD</t>
-  </si>
-  <si>
-    <t>Configuration</t>
-  </si>
-  <si>
-    <t>CL</t>
-  </si>
-  <si>
-    <t>CD</t>
-  </si>
-  <si>
-    <t>Pitch Front</t>
-  </si>
-  <si>
-    <t>Pitch Rear</t>
   </si>
 </sst>
 </file>
@@ -1042,8 +1042,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1056,19 +1056,19 @@
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="23" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="C1" s="25" t="s">
         <v>44</v>
       </c>
-      <c r="B1" s="24" t="s">
+      <c r="D1" s="25" t="s">
         <v>45</v>
       </c>
-      <c r="C1" s="25" t="s">
+      <c r="E1" s="26" t="s">
         <v>46</v>
-      </c>
-      <c r="D1" s="25" t="s">
-        <v>47</v>
-      </c>
-      <c r="E1" s="26" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -1079,10 +1079,10 @@
         <v>1</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E2" s="11"/>
     </row>
@@ -1092,10 +1092,10 @@
         <v>2</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D3" s="14" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E3" s="15"/>
     </row>
@@ -1126,7 +1126,7 @@
         <v>7</v>
       </c>
       <c r="E5" s="15" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1155,10 +1155,10 @@
         <v>1.44</v>
       </c>
       <c r="D7" s="19" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E7" s="20" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -1166,63 +1166,63 @@
         <v>13</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C8" s="9">
         <v>-2.75</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E8" s="11" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="36"/>
       <c r="B9" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C9" s="4">
         <v>-1.0900000000000001</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E9" s="21" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="36"/>
       <c r="B10" s="2" t="s">
-        <v>20</v>
+        <v>104</v>
       </c>
       <c r="C10" s="4">
         <v>1</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E10" s="21"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="36"/>
       <c r="B11" s="2" t="s">
-        <v>21</v>
+        <v>105</v>
       </c>
       <c r="C11" s="4">
         <v>1</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E11" s="21"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="36"/>
       <c r="B12" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C12" s="4">
         <v>33.700000000000003</v>
@@ -1248,7 +1248,7 @@
     <row r="14" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="35"/>
       <c r="B14" s="12" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C14" s="13">
         <v>1.2250000000000001</v>
@@ -1257,7 +1257,7 @@
         <v>18</v>
       </c>
       <c r="E14" s="15" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -1265,7 +1265,7 @@
         <v>19</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C15" s="9">
         <v>39.700000000000003</v>
@@ -1274,13 +1274,13 @@
         <v>8</v>
       </c>
       <c r="E15" s="11" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="36"/>
       <c r="B16" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C16" s="4">
         <v>26.84</v>
@@ -1289,43 +1289,43 @@
         <v>8</v>
       </c>
       <c r="E16" s="21" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="36"/>
       <c r="B17" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C17" s="4">
         <v>0.41</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E17" s="21" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="36"/>
       <c r="B18" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C18" s="4">
         <v>4</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E18" s="21" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="36"/>
       <c r="B19" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C19" s="4">
         <v>25.4</v>
@@ -1334,13 +1334,13 @@
         <v>8</v>
       </c>
       <c r="E19" s="21" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="36"/>
       <c r="B20" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C20" s="4">
         <v>15.88</v>
@@ -1349,43 +1349,43 @@
         <v>8</v>
       </c>
       <c r="E20" s="21" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="35"/>
       <c r="B21" s="12" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C21" s="13">
         <v>2.82</v>
       </c>
       <c r="D21" s="14" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E21" s="15" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="34" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C22" s="9">
         <v>1</v>
       </c>
       <c r="D22" s="10" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E22" s="11"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="36"/>
       <c r="B23" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C23" s="4">
         <v>203.2</v>
@@ -1394,43 +1394,43 @@
         <v>8</v>
       </c>
       <c r="E23" s="21" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="36"/>
       <c r="B24" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C24" s="4">
         <v>-1E-3</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E24" s="21" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="36"/>
       <c r="B25" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C25" s="4">
         <v>2</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E25" s="21" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="36"/>
       <c r="B26" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C26" s="4">
         <v>250</v>
@@ -1439,43 +1439,43 @@
         <v>6</v>
       </c>
       <c r="E26" s="21" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="36"/>
       <c r="B27" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C27" s="4">
         <v>1E-4</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E27" s="21" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="36"/>
       <c r="B28" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C28" s="4">
         <v>1.8</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E28" s="21" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="36"/>
       <c r="B29" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C29" s="4">
         <v>250</v>
@@ -1484,311 +1484,311 @@
         <v>6</v>
       </c>
       <c r="E29" s="21" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="36"/>
       <c r="B30" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C30" s="4">
         <v>1E-4</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E30" s="21" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="36"/>
       <c r="B31" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C31" s="4">
         <v>800</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E31" s="21" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="35"/>
       <c r="B32" s="12" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C32" s="13">
         <v>1000</v>
       </c>
       <c r="D32" s="14" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E32" s="15" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="34" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B33" s="8" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C33" s="9">
         <v>1</v>
       </c>
       <c r="D33" s="10" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E33" s="11"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="36"/>
       <c r="B34" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C34" s="4">
         <v>1</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E34" s="21" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="35"/>
       <c r="B35" s="12" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C35" s="22">
         <v>1</v>
       </c>
       <c r="D35" s="14" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E35" s="15" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="31" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B36" s="8" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C36" s="9" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D36" s="10" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E36" s="11"/>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="32"/>
       <c r="B37" s="5" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C37" s="6">
         <v>1</v>
       </c>
       <c r="D37" s="7" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E37" s="29" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="32"/>
       <c r="B38" s="5" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C38" s="6">
         <v>0.98</v>
       </c>
       <c r="D38" s="7" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E38" s="29" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="32"/>
       <c r="B39" s="5" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C39" s="6">
         <v>0.98</v>
       </c>
       <c r="D39" s="7" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E39" s="29" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="32"/>
       <c r="B40" s="5" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C40" s="6">
         <v>0.98</v>
       </c>
       <c r="D40" s="7" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E40" s="29" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="32"/>
       <c r="B41" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C41" s="4">
         <v>1</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E41" s="21" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="32"/>
       <c r="B42" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C42" s="30">
         <v>1</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E42" s="21"/>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="32"/>
       <c r="B43" s="27" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C43" s="4">
         <v>12.9</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E43" s="21"/>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="32"/>
       <c r="B44" s="27" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C44" s="4"/>
       <c r="D44" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E44" s="21"/>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="32"/>
       <c r="B45" s="27" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C45" s="4"/>
       <c r="D45" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E45" s="21"/>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="32"/>
       <c r="B46" s="27" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C46" s="4"/>
       <c r="D46" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E46" s="21"/>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="32"/>
       <c r="B47" s="27" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C47" s="4"/>
       <c r="D47" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E47" s="21"/>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="32"/>
       <c r="B48" s="27" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C48" s="4"/>
       <c r="D48" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E48" s="21"/>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="32"/>
       <c r="B49" s="27" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C49" s="4"/>
       <c r="D49" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E49" s="21"/>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="32"/>
       <c r="B50" s="27" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C50" s="4"/>
       <c r="D50" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E50" s="21"/>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="32"/>
       <c r="B51" s="27" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C51" s="4"/>
       <c r="D51" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E51" s="21"/>
     </row>
     <row r="52" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="33"/>
       <c r="B52" s="28" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C52" s="13"/>
       <c r="D52" s="14" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E52" s="15"/>
     </row>
@@ -2387,19 +2387,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C1" t="s">
         <v>101</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>102</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>103</v>
-      </c>
-      <c r="D1" t="s">
-        <v>104</v>
-      </c>
-      <c r="E1" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>